<commit_message>
DOCs: new sheet, inputFile
</commit_message>
<xml_diff>
--- a/CW_ThoughtsOutLoud/Documents/Примеры справочников.xlsx
+++ b/CW_ThoughtsOutLoud/Documents/Примеры справочников.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fosti\source\repos\Fostiriy\University\CW_ThoughtsOutLoud\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27DC161F-7F29-4AB8-A881-EDD682CCD597}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89EDB47F-73FD-46C6-AC87-0973D5A11380}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="348" windowWidth="23256" windowHeight="12720" xr2:uid="{A80E80F6-15F0-443C-827D-E94124B27E61}"/>
+    <workbookView xWindow="-108" yWindow="348" windowWidth="23256" windowHeight="12720" activeTab="2" xr2:uid="{A80E80F6-15F0-443C-827D-E94124B27E61}"/>
   </bookViews>
   <sheets>
-    <sheet name="Лист1" sheetId="1" r:id="rId1"/>
+    <sheet name="Справочник имя-дата-время" sheetId="1" r:id="rId1"/>
+    <sheet name="Справочник категория-цвет" sheetId="2" r:id="rId2"/>
+    <sheet name="Лист2" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,17 +36,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="30">
   <si>
     <t>Имя аудиозаписи</t>
   </si>
   <si>
-    <t>Дата записи</t>
-  </si>
-  <si>
-    <t>Время записи</t>
-  </si>
-  <si>
     <t>Лекция 1</t>
   </si>
   <si>
@@ -64,6 +60,72 @@
   </si>
   <si>
     <t>История_друга</t>
+  </si>
+  <si>
+    <t>Планы на будущее</t>
+  </si>
+  <si>
+    <t>Категория1</t>
+  </si>
+  <si>
+    <t>Категория2</t>
+  </si>
+  <si>
+    <t>Музыка</t>
+  </si>
+  <si>
+    <t>Стихи</t>
+  </si>
+  <si>
+    <t>Истории</t>
+  </si>
+  <si>
+    <t>Матанализ</t>
+  </si>
+  <si>
+    <t>Цвет категории</t>
+  </si>
+  <si>
+    <t>Красный</t>
+  </si>
+  <si>
+    <t>Чёрный</t>
+  </si>
+  <si>
+    <t>Синий</t>
+  </si>
+  <si>
+    <t>Зелёный</t>
+  </si>
+  <si>
+    <t>Жёлтый</t>
+  </si>
+  <si>
+    <t>Геометрия</t>
+  </si>
+  <si>
+    <t>ФСДиА</t>
+  </si>
+  <si>
+    <t>Избранное</t>
+  </si>
+  <si>
+    <t>Без категории</t>
+  </si>
+  <si>
+    <t>Белый</t>
+  </si>
+  <si>
+    <t>Фиолетовый</t>
+  </si>
+  <si>
+    <t>Дата и время записи</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Музыка </t>
+  </si>
+  <si>
+    <t>Категория</t>
   </si>
 </sst>
 </file>
@@ -103,7 +165,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -126,11 +188,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -138,6 +237,20 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="21" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="22" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -452,33 +565,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C719CDF-33D0-4D02-8D2D-2F2B60178BC7}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.77734375" customWidth="1"/>
-    <col min="3" max="3" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" customWidth="1"/>
+    <col min="6" max="6" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="B1" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="7"/>
     </row>
     <row r="2" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B2" s="3">
         <v>43180</v>
@@ -489,7 +601,7 @@
     </row>
     <row r="3" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B3" s="3">
         <v>44170</v>
@@ -500,7 +612,7 @@
     </row>
     <row r="4" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B4" s="3">
         <v>43180</v>
@@ -511,7 +623,7 @@
     </row>
     <row r="5" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B5" s="3">
         <v>44345</v>
@@ -522,7 +634,7 @@
     </row>
     <row r="6" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B6" s="3">
         <v>43500</v>
@@ -533,7 +645,7 @@
     </row>
     <row r="7" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B7" s="3">
         <v>44177</v>
@@ -544,7 +656,7 @@
     </row>
     <row r="8" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B8" s="3">
         <v>44200</v>
@@ -555,7 +667,7 @@
     </row>
     <row r="9" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B9" s="3">
         <v>44313</v>
@@ -566,17 +678,314 @@
     </row>
     <row r="10" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B10" s="3">
         <v>44312</v>
       </c>
       <c r="C10" s="4">
         <v>0.35413194444444446</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+      <c r="A11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="3">
+        <v>42942</v>
+      </c>
+      <c r="C11" s="4">
+        <v>0.57343749999999993</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:C1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{956F8B78-5030-48E6-91E8-2522336EEF23}">
+  <dimension ref="A1:B11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A8" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A11" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCAAAE3F-A587-4D06-9374-2DADEBE5BB7C}">
+  <dimension ref="A1:D11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="A2" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="8">
+        <v>43180.632476851853</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="A3" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="8">
+        <v>44170.888877314814</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="A4" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="8">
+        <v>43180.702256944445</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="A5" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="8">
+        <v>44345.023634259262</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="A6" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="8">
+        <v>43500.468657407408</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="A7" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="8">
+        <v>44177.808194444442</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="A8" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="8">
+        <v>44200.699953703705</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="A9" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="8">
+        <v>44313.414027777777</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="A10" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="8">
+        <v>44313.414027777777</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="A11" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="8">
+        <v>44312.354131944441</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Big problems when testing were fixed in HT and RBTree
</commit_message>
<xml_diff>
--- a/CW_ThoughtsOutLoud/Documents/Примеры справочников.xlsx
+++ b/CW_ThoughtsOutLoud/Documents/Примеры справочников.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fosti\source\repos\Fostiriy\University\CW_ThoughtsOutLoud\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89EDB47F-73FD-46C6-AC87-0973D5A11380}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{404BB414-B7C8-40BB-9400-D71EF761738D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="348" windowWidth="23256" windowHeight="12720" activeTab="2" xr2:uid="{A80E80F6-15F0-443C-827D-E94124B27E61}"/>
+    <workbookView xWindow="-108" yWindow="348" windowWidth="23256" windowHeight="12720" xr2:uid="{A80E80F6-15F0-443C-827D-E94124B27E61}"/>
   </bookViews>
   <sheets>
-    <sheet name="Справочник имя-дата-время" sheetId="1" r:id="rId1"/>
-    <sheet name="Справочник категория-цвет" sheetId="2" r:id="rId2"/>
-    <sheet name="Лист2" sheetId="3" r:id="rId3"/>
+    <sheet name="Все метаданные" sheetId="3" r:id="rId1"/>
+    <sheet name="Справочник имя-дата-время" sheetId="1" r:id="rId2"/>
+    <sheet name="Справочник категория-цвет" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -132,6 +132,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy\ h:mm:ss"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -229,7 +232,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -238,12 +241,6 @@
     <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="21" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="22" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -251,6 +248,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -564,11 +568,187 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCAAAE3F-A587-4D06-9374-2DADEBE5BB7C}">
+  <dimension ref="A1:D11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D10" activeCellId="2" sqref="A10 C10 D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.5546875" customWidth="1"/>
+    <col min="3" max="3" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="A2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="11">
+        <v>43180.632476851853</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="A3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="11">
+        <v>44170.888877314814</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="A4" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="11">
+        <v>43180.702256944445</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="A5" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="11">
+        <v>44345.023634259262</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="A6" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="11">
+        <v>43500.468657407408</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="A7" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="11">
+        <v>44177.808194444442</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="A8" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="11">
+        <v>44200.699953703705</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="A9" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="11">
+        <v>44313.414027777777</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="A10" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="11">
+        <v>44313.414027777777</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="A11" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="11">
+        <v>44312.354131944441</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C719CDF-33D0-4D02-8D2D-2F2B60178BC7}">
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -583,10 +763,10 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="7"/>
+      <c r="C1" s="10"/>
     </row>
     <row r="2" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
@@ -707,7 +887,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{956F8B78-5030-48E6-91E8-2522336EEF23}">
   <dimension ref="A1:B11"/>
   <sheetViews>
@@ -813,179 +993,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCAAAE3F-A587-4D06-9374-2DADEBE5BB7C}">
-  <dimension ref="A1:D11"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.6640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="C1" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.35">
-      <c r="A2" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="8">
-        <v>43180.632476851853</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="18" x14ac:dyDescent="0.35">
-      <c r="A3" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="8">
-        <v>44170.888877314814</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="18" x14ac:dyDescent="0.35">
-      <c r="A4" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="8">
-        <v>43180.702256944445</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="18" x14ac:dyDescent="0.35">
-      <c r="A5" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="8">
-        <v>44345.023634259262</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="18" x14ac:dyDescent="0.35">
-      <c r="A6" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="8">
-        <v>43500.468657407408</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="18" x14ac:dyDescent="0.35">
-      <c r="A7" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="8">
-        <v>44177.808194444442</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="18" x14ac:dyDescent="0.35">
-      <c r="A8" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="8">
-        <v>44200.699953703705</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="18" x14ac:dyDescent="0.35">
-      <c r="A9" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" s="8">
-        <v>44313.414027777777</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="18" x14ac:dyDescent="0.35">
-      <c r="A10" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10" s="8">
-        <v>44313.414027777777</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="18" x14ac:dyDescent="0.35">
-      <c r="A11" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B11" s="8">
-        <v>44312.354131944441</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>25</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>